<commit_message>
adding two new KPIs (posm fsos and lsos) to pnghk
</commit_message>
<xml_diff>
--- a/Projects/PNGHK/Data/09_PNGHK_template_2019_07_30.xlsx
+++ b/Projects/PNGHK/Data/09_PNGHK_template_2019_07_30.xlsx
@@ -19,6 +19,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">KPIS!$A$1:$V$105</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">KPIS!$A$1:$V$105</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">KPIS!$A$1:$V$105</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">KPIS!$A$1:$V$105</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2313" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2315" uniqueCount="152">
   <si>
     <t xml:space="preserve">KPI_ID</t>
   </si>
@@ -495,7 +496,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -545,6 +546,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -640,7 +646,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -714,19 +720,27 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -749,7 +763,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -840,15 +854,13 @@
   </sheetPr>
   <dimension ref="A1:AI107"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A103" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A107" activeCellId="0" sqref="106:107"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B104" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J105" activeCellId="0" sqref="J105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="76.4030612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="75.5969387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8705,21 +8717,24 @@
       <c r="AH105" s="4"/>
       <c r="AI105" s="4"/>
     </row>
-    <row r="106" customFormat="false" ht="91.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" s="21" customFormat="true" ht="91.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="18" t="n">
         <v>31</v>
       </c>
       <c r="B106" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C106" s="5" t="s">
+      <c r="C106" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="D106" s="19" t="s">
+      <c r="D106" s="20" t="s">
         <v>24</v>
       </c>
+      <c r="E106" s="21" t="s">
+        <v>91</v>
+      </c>
       <c r="F106" s="18"/>
-      <c r="H106" s="20" t="s">
+      <c r="H106" s="22" t="s">
         <v>25</v>
       </c>
       <c r="I106" s="18" t="s">
@@ -8737,8 +8752,8 @@
       <c r="M106" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="N106" s="21" t="s">
-        <v>26</v>
+      <c r="N106" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="O106" s="18" t="s">
         <v>26</v>
@@ -8746,7 +8761,7 @@
       <c r="P106" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="Q106" s="20" t="s">
+      <c r="Q106" s="22" t="s">
         <v>39</v>
       </c>
       <c r="S106" s="18" t="s">
@@ -8762,21 +8777,24 @@
         <v>119</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="91.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" s="21" customFormat="true" ht="102.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="18" t="n">
         <v>32</v>
       </c>
       <c r="B107" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C107" s="5" t="s">
+      <c r="C107" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="D107" s="19" t="s">
+      <c r="D107" s="20" t="s">
         <v>24</v>
       </c>
+      <c r="E107" s="23" t="s">
+        <v>91</v>
+      </c>
       <c r="F107" s="18"/>
-      <c r="H107" s="20" t="s">
+      <c r="H107" s="22" t="s">
         <v>25</v>
       </c>
       <c r="I107" s="18" t="s">
@@ -8794,8 +8812,8 @@
       <c r="M107" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="N107" s="21" t="s">
-        <v>26</v>
+      <c r="N107" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="O107" s="18" t="s">
         <v>26</v>
@@ -8803,7 +8821,7 @@
       <c r="P107" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="Q107" s="20" t="s">
+      <c r="Q107" s="22" t="s">
         <v>39</v>
       </c>
       <c r="S107" s="18" t="s">
@@ -8846,19 +8864,16 @@
   <dimension ref="A1:L60"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="1" sqref="106:107 F10"/>
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.9795918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.4387755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.0714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="52" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8886,7 +8901,7 @@
       <c r="H1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="I1" s="24" t="s">
         <v>130</v>
       </c>
     </row>
@@ -8894,22 +8909,22 @@
       <c r="A2" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="E2" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="F2" s="23" t="n">
+      <c r="E2" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="F2" s="25" t="n">
         <v>7</v>
       </c>
-      <c r="G2" s="25"/>
+      <c r="G2" s="27"/>
       <c r="I2" s="0" t="s">
         <v>134</v>
       </c>
@@ -8918,19 +8933,19 @@
       <c r="A3" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="D3" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E3" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G3" s="26"/>
+      <c r="D3" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G3" s="28"/>
       <c r="I3" s="0" t="s">
         <v>135</v>
       </c>
@@ -8939,19 +8954,19 @@
       <c r="A4" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="D4" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E4" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G4" s="26"/>
+      <c r="D4" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G4" s="28"/>
       <c r="I4" s="0" t="s">
         <v>135</v>
       </c>
@@ -8960,22 +8975,22 @@
       <c r="A5" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="E5" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="F5" s="23" t="n">
+      <c r="E5" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="F5" s="25" t="n">
         <v>6</v>
       </c>
-      <c r="G5" s="25"/>
+      <c r="G5" s="27"/>
       <c r="I5" s="0" t="s">
         <v>134</v>
       </c>
@@ -8984,19 +8999,19 @@
       <c r="A6" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="D6" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G6" s="26"/>
+      <c r="D6" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G6" s="28"/>
       <c r="I6" s="0" t="s">
         <v>135</v>
       </c>
@@ -9005,19 +9020,19 @@
       <c r="A7" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="D7" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E7" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G7" s="26"/>
+      <c r="D7" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G7" s="28"/>
       <c r="I7" s="0" t="s">
         <v>135</v>
       </c>
@@ -9026,22 +9041,22 @@
       <c r="A8" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="E8" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="F8" s="23" t="n">
+      <c r="E8" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="F8" s="25" t="n">
         <v>5</v>
       </c>
-      <c r="G8" s="25"/>
+      <c r="G8" s="27"/>
       <c r="I8" s="0" t="s">
         <v>134</v>
       </c>
@@ -9050,22 +9065,22 @@
       <c r="A9" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="E9" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="F9" s="23" t="n">
+      <c r="E9" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="F9" s="25" t="n">
         <v>5</v>
       </c>
-      <c r="G9" s="25"/>
+      <c r="G9" s="27"/>
       <c r="I9" s="0" t="s">
         <v>135</v>
       </c>
@@ -9074,20 +9089,20 @@
       <c r="A10" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="D10" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E10" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="F10" s="23"/>
-      <c r="G10" s="25"/>
+      <c r="D10" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="F10" s="25"/>
+      <c r="G10" s="27"/>
       <c r="I10" s="0" t="s">
         <v>135</v>
       </c>
@@ -9096,22 +9111,22 @@
       <c r="A11" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="E11" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="F11" s="23" t="n">
+      <c r="E11" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="F11" s="25" t="n">
         <v>7</v>
       </c>
-      <c r="G11" s="25"/>
+      <c r="G11" s="27"/>
       <c r="I11" s="0" t="s">
         <v>134</v>
       </c>
@@ -9120,20 +9135,20 @@
       <c r="A12" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="D12" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="F12" s="23"/>
-      <c r="G12" s="25"/>
+      <c r="D12" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="F12" s="25"/>
+      <c r="G12" s="27"/>
       <c r="I12" s="0" t="s">
         <v>135</v>
       </c>
@@ -9142,19 +9157,19 @@
       <c r="A13" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="D13" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E13" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G13" s="26"/>
+      <c r="D13" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G13" s="28"/>
       <c r="I13" s="0" t="s">
         <v>135</v>
       </c>
@@ -9163,19 +9178,19 @@
       <c r="A14" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="D14" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G14" s="26"/>
+      <c r="D14" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G14" s="28"/>
       <c r="I14" s="0" t="s">
         <v>135</v>
       </c>
@@ -9184,337 +9199,337 @@
       <c r="A15" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="D15" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E15" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G15" s="26"/>
+      <c r="D15" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G15" s="28"/>
       <c r="I15" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="L15" s="27"/>
+      <c r="L15" s="29"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="D16" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G16" s="26"/>
+      <c r="D16" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E16" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G16" s="28"/>
       <c r="I16" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="L16" s="27"/>
+      <c r="L16" s="29"/>
     </row>
     <row r="17" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C17" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="D17" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E17" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G17" s="26"/>
+      <c r="D17" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G17" s="28"/>
       <c r="I17" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="L17" s="27"/>
+      <c r="L17" s="29"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="D18" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E18" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G18" s="26"/>
+      <c r="D18" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G18" s="28"/>
       <c r="I18" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="L18" s="27"/>
+      <c r="L18" s="29"/>
     </row>
     <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="C19" s="24" t="s">
+      <c r="C19" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="D19" s="23" t="s">
+      <c r="D19" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="E19" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G19" s="23" t="s">
+      <c r="E19" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G19" s="25" t="s">
         <v>148</v>
       </c>
       <c r="I19" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="L19" s="27"/>
+      <c r="L19" s="29"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="C20" s="24" t="s">
+      <c r="C20" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="D20" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E20" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G20" s="28"/>
+      <c r="D20" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G20" s="30"/>
       <c r="I20" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="L20" s="27"/>
+      <c r="L20" s="29"/>
     </row>
     <row r="21" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="C21" s="24" t="s">
+      <c r="C21" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="D21" s="23" t="s">
+      <c r="D21" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="E21" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G21" s="23" t="s">
+      <c r="E21" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G21" s="25" t="s">
         <v>148</v>
       </c>
       <c r="I21" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="L21" s="27"/>
+      <c r="L21" s="29"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="C22" s="24" t="s">
+      <c r="C22" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="D22" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E22" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G22" s="28"/>
+      <c r="D22" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G22" s="30"/>
       <c r="I22" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="L22" s="27"/>
+      <c r="L22" s="29"/>
     </row>
     <row r="23" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="C23" s="24" t="s">
+      <c r="C23" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="D23" s="23" t="s">
+      <c r="D23" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="E23" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G23" s="23" t="s">
+      <c r="E23" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G23" s="25" t="s">
         <v>148</v>
       </c>
       <c r="I23" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="L23" s="27"/>
+      <c r="L23" s="29"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="C24" s="24" t="s">
+      <c r="C24" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="D24" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E24" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G24" s="28"/>
+      <c r="D24" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E24" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G24" s="30"/>
       <c r="I24" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="L24" s="27"/>
+      <c r="L24" s="29"/>
     </row>
     <row r="25" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="C25" s="24" t="s">
+      <c r="C25" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="D25" s="23" t="s">
+      <c r="D25" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="E25" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G25" s="23" t="s">
+      <c r="E25" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G25" s="25" t="s">
         <v>148</v>
       </c>
       <c r="I25" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="L25" s="27"/>
+      <c r="L25" s="29"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="C26" s="24" t="s">
+      <c r="C26" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="D26" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E26" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G26" s="28"/>
+      <c r="D26" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E26" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G26" s="30"/>
       <c r="I26" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="L26" s="27"/>
+      <c r="L26" s="29"/>
     </row>
     <row r="27" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="B27" s="23" t="s">
+      <c r="B27" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="C27" s="24" t="s">
+      <c r="C27" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="D27" s="23" t="s">
+      <c r="D27" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="E27" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G27" s="23" t="s">
+      <c r="E27" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G27" s="25" t="s">
         <v>148</v>
       </c>
       <c r="I27" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="L27" s="27"/>
+      <c r="L27" s="29"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="B28" s="23" t="s">
+      <c r="B28" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="C28" s="24" t="s">
+      <c r="C28" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="D28" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E28" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G28" s="28"/>
+      <c r="D28" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E28" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G28" s="30"/>
       <c r="I28" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="L28" s="27"/>
+      <c r="L28" s="29"/>
     </row>
     <row r="29" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="B29" s="23" t="s">
+      <c r="B29" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="C29" s="24" t="s">
+      <c r="C29" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="D29" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E29" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G29" s="28"/>
+      <c r="D29" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E29" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G29" s="30"/>
       <c r="I29" s="0" t="s">
         <v>135</v>
       </c>
@@ -9523,19 +9538,19 @@
       <c r="A30" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="23" t="s">
+      <c r="B30" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="C30" s="24" t="s">
+      <c r="C30" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="D30" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E30" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G30" s="28"/>
+      <c r="D30" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E30" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G30" s="30"/>
       <c r="I30" s="0" t="s">
         <v>135</v>
       </c>
@@ -9544,19 +9559,19 @@
       <c r="A31" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B31" s="23" t="s">
+      <c r="B31" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="C31" s="24" t="s">
+      <c r="C31" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="D31" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E31" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G31" s="28"/>
+      <c r="D31" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E31" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G31" s="30"/>
       <c r="I31" s="0" t="s">
         <v>135</v>
       </c>
@@ -9565,19 +9580,19 @@
       <c r="A32" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B32" s="23" t="s">
+      <c r="B32" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="C32" s="24" t="s">
+      <c r="C32" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="D32" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E32" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G32" s="28"/>
+      <c r="D32" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E32" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G32" s="30"/>
       <c r="I32" s="0" t="s">
         <v>135</v>
       </c>
@@ -9586,19 +9601,19 @@
       <c r="A33" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="B33" s="23" t="s">
+      <c r="B33" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="C33" s="24" t="s">
+      <c r="C33" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="D33" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E33" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G33" s="26"/>
+      <c r="D33" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E33" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G33" s="28"/>
       <c r="I33" s="0" t="s">
         <v>134</v>
       </c>
@@ -9607,19 +9622,19 @@
       <c r="A34" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="B34" s="23" t="s">
+      <c r="B34" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="C34" s="24" t="s">
+      <c r="C34" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="D34" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E34" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G34" s="26"/>
+      <c r="D34" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E34" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G34" s="28"/>
       <c r="I34" s="0" t="s">
         <v>135</v>
       </c>
@@ -9628,19 +9643,19 @@
       <c r="A35" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B35" s="23" t="s">
+      <c r="B35" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="C35" s="24" t="s">
+      <c r="C35" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="D35" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E35" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G35" s="26"/>
+      <c r="D35" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E35" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G35" s="28"/>
       <c r="I35" s="0" t="s">
         <v>134</v>
       </c>
@@ -9649,19 +9664,19 @@
       <c r="A36" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B36" s="23" t="s">
+      <c r="B36" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="C36" s="24" t="s">
+      <c r="C36" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="D36" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E36" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G36" s="26"/>
+      <c r="D36" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E36" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G36" s="28"/>
       <c r="I36" s="0" t="s">
         <v>135</v>
       </c>
@@ -9670,19 +9685,19 @@
       <c r="A37" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="B37" s="23" t="s">
+      <c r="B37" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="C37" s="24" t="s">
+      <c r="C37" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="D37" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E37" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G37" s="26"/>
+      <c r="D37" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E37" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G37" s="28"/>
       <c r="I37" s="0" t="s">
         <v>134</v>
       </c>
@@ -9691,19 +9706,19 @@
       <c r="A38" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="B38" s="23" t="s">
+      <c r="B38" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="C38" s="24" t="s">
+      <c r="C38" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="D38" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E38" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G38" s="26"/>
+      <c r="D38" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E38" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G38" s="28"/>
       <c r="I38" s="0" t="s">
         <v>135</v>
       </c>
@@ -9712,19 +9727,19 @@
       <c r="A39" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B39" s="23" t="s">
+      <c r="B39" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="C39" s="24" t="s">
+      <c r="C39" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="D39" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E39" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G39" s="26"/>
+      <c r="D39" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E39" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G39" s="28"/>
       <c r="I39" s="0" t="s">
         <v>134</v>
       </c>
@@ -9733,19 +9748,19 @@
       <c r="A40" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B40" s="23" t="s">
+      <c r="B40" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="C40" s="24" t="s">
+      <c r="C40" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="D40" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E40" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G40" s="26"/>
+      <c r="D40" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E40" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G40" s="28"/>
       <c r="I40" s="0" t="s">
         <v>135</v>
       </c>
@@ -9754,19 +9769,19 @@
       <c r="A41" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="C41" s="24" t="s">
+      <c r="C41" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="D41" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E41" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G41" s="26"/>
+      <c r="D41" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E41" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G41" s="28"/>
       <c r="I41" s="0" t="s">
         <v>134</v>
       </c>
@@ -9775,19 +9790,19 @@
       <c r="A42" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="B42" s="23" t="s">
+      <c r="B42" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="C42" s="24" t="s">
+      <c r="C42" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="D42" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E42" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G42" s="26"/>
+      <c r="D42" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E42" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G42" s="28"/>
       <c r="I42" s="0" t="s">
         <v>135</v>
       </c>
@@ -9796,19 +9811,19 @@
       <c r="A43" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="B43" s="23" t="s">
+      <c r="B43" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="C43" s="24" t="s">
+      <c r="C43" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="D43" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E43" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G43" s="26"/>
+      <c r="D43" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E43" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G43" s="28"/>
       <c r="I43" s="0" t="s">
         <v>134</v>
       </c>
@@ -9817,19 +9832,19 @@
       <c r="A44" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="B44" s="23" t="s">
+      <c r="B44" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="C44" s="24" t="s">
+      <c r="C44" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="D44" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E44" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G44" s="26"/>
+      <c r="D44" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E44" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G44" s="28"/>
       <c r="I44" s="0" t="s">
         <v>135</v>
       </c>
@@ -9838,19 +9853,19 @@
       <c r="A45" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B45" s="23" t="s">
+      <c r="B45" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="C45" s="24" t="s">
+      <c r="C45" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="D45" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E45" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G45" s="26"/>
+      <c r="D45" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E45" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G45" s="28"/>
       <c r="I45" s="0" t="s">
         <v>134</v>
       </c>
@@ -9859,19 +9874,19 @@
       <c r="A46" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B46" s="23" t="s">
+      <c r="B46" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="C46" s="24" t="s">
+      <c r="C46" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="D46" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E46" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G46" s="26"/>
+      <c r="D46" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E46" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G46" s="28"/>
       <c r="I46" s="0" t="s">
         <v>135</v>
       </c>
@@ -9880,19 +9895,19 @@
       <c r="A47" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="B47" s="23" t="s">
+      <c r="B47" s="25" t="s">
         <v>150</v>
       </c>
-      <c r="C47" s="24" t="s">
+      <c r="C47" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="D47" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E47" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G47" s="28"/>
+      <c r="D47" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E47" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G47" s="30"/>
       <c r="I47" s="0" t="s">
         <v>134</v>
       </c>
@@ -9901,19 +9916,19 @@
       <c r="A48" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="B48" s="23" t="s">
+      <c r="B48" s="25" t="s">
         <v>150</v>
       </c>
-      <c r="C48" s="24" t="s">
+      <c r="C48" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="D48" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E48" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G48" s="28"/>
+      <c r="D48" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E48" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G48" s="30"/>
       <c r="I48" s="0" t="s">
         <v>135</v>
       </c>
@@ -9922,19 +9937,19 @@
       <c r="A49" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B49" s="23" t="s">
+      <c r="B49" s="25" t="s">
         <v>150</v>
       </c>
-      <c r="C49" s="24" t="s">
+      <c r="C49" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="D49" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E49" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G49" s="28"/>
+      <c r="D49" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E49" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G49" s="30"/>
       <c r="I49" s="0" t="s">
         <v>134</v>
       </c>
@@ -9943,19 +9958,19 @@
       <c r="A50" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B50" s="23" t="s">
+      <c r="B50" s="25" t="s">
         <v>150</v>
       </c>
-      <c r="C50" s="24" t="s">
+      <c r="C50" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="D50" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E50" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G50" s="28"/>
+      <c r="D50" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E50" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G50" s="30"/>
       <c r="I50" s="0" t="s">
         <v>135</v>
       </c>
@@ -9964,20 +9979,20 @@
       <c r="A51" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="B51" s="23" t="s">
+      <c r="B51" s="25" t="s">
         <v>150</v>
       </c>
-      <c r="C51" s="24" t="s">
+      <c r="C51" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="D51" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E51" s="23" t="s">
+      <c r="D51" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E51" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="G51" s="28"/>
-      <c r="H51" s="23" t="s">
+      <c r="G51" s="30"/>
+      <c r="H51" s="25" t="s">
         <v>151</v>
       </c>
       <c r="I51" s="0" t="s">
@@ -9988,19 +10003,19 @@
       <c r="A52" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="B52" s="23" t="s">
+      <c r="B52" s="25" t="s">
         <v>150</v>
       </c>
-      <c r="C52" s="24" t="s">
+      <c r="C52" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="D52" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E52" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G52" s="28"/>
+      <c r="D52" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E52" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G52" s="30"/>
       <c r="I52" s="0" t="s">
         <v>135</v>
       </c>
@@ -10009,20 +10024,20 @@
       <c r="A53" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B53" s="23" t="s">
+      <c r="B53" s="25" t="s">
         <v>150</v>
       </c>
-      <c r="C53" s="24" t="s">
+      <c r="C53" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="D53" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E53" s="23" t="s">
+      <c r="D53" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E53" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="G53" s="28"/>
-      <c r="H53" s="23" t="s">
+      <c r="G53" s="30"/>
+      <c r="H53" s="25" t="s">
         <v>151</v>
       </c>
       <c r="I53" s="0" t="s">
@@ -10033,19 +10048,19 @@
       <c r="A54" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B54" s="23" t="s">
+      <c r="B54" s="25" t="s">
         <v>150</v>
       </c>
-      <c r="C54" s="24" t="s">
+      <c r="C54" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="D54" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E54" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G54" s="28"/>
+      <c r="D54" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E54" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G54" s="30"/>
       <c r="I54" s="0" t="s">
         <v>135</v>
       </c>
@@ -10054,19 +10069,19 @@
       <c r="A55" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="B55" s="23" t="s">
+      <c r="B55" s="25" t="s">
         <v>150</v>
       </c>
-      <c r="C55" s="24" t="s">
+      <c r="C55" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="D55" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E55" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G55" s="28"/>
+      <c r="D55" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E55" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G55" s="30"/>
       <c r="I55" s="0" t="s">
         <v>134</v>
       </c>
@@ -10075,19 +10090,19 @@
       <c r="A56" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="B56" s="23" t="s">
+      <c r="B56" s="25" t="s">
         <v>150</v>
       </c>
-      <c r="C56" s="24" t="s">
+      <c r="C56" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="D56" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E56" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G56" s="28"/>
+      <c r="D56" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E56" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G56" s="30"/>
       <c r="I56" s="0" t="s">
         <v>135</v>
       </c>
@@ -10096,19 +10111,19 @@
       <c r="A57" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="B57" s="23" t="s">
+      <c r="B57" s="25" t="s">
         <v>150</v>
       </c>
-      <c r="C57" s="24" t="s">
+      <c r="C57" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="D57" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E57" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G57" s="28"/>
+      <c r="D57" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E57" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G57" s="30"/>
       <c r="I57" s="0" t="s">
         <v>134</v>
       </c>
@@ -10117,19 +10132,19 @@
       <c r="A58" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="B58" s="23" t="s">
+      <c r="B58" s="25" t="s">
         <v>150</v>
       </c>
-      <c r="C58" s="24" t="s">
+      <c r="C58" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="D58" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E58" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G58" s="28"/>
+      <c r="D58" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E58" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G58" s="30"/>
       <c r="I58" s="0" t="s">
         <v>135</v>
       </c>
@@ -10138,19 +10153,19 @@
       <c r="A59" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B59" s="23" t="s">
+      <c r="B59" s="25" t="s">
         <v>150</v>
       </c>
-      <c r="C59" s="24" t="s">
+      <c r="C59" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="D59" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E59" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G59" s="28"/>
+      <c r="D59" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E59" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G59" s="30"/>
       <c r="I59" s="0" t="s">
         <v>134</v>
       </c>
@@ -10159,19 +10174,19 @@
       <c r="A60" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B60" s="23" t="s">
+      <c r="B60" s="25" t="s">
         <v>150</v>
       </c>
-      <c r="C60" s="24" t="s">
+      <c r="C60" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="D60" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E60" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G60" s="28"/>
+      <c r="D60" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E60" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G60" s="30"/>
       <c r="I60" s="0" t="s">
         <v>135</v>
       </c>

</xml_diff>